<commit_message>
better weibull axis formatting
</commit_message>
<xml_diff>
--- a/Fibre_data_V3.xlsx
+++ b/Fibre_data_V3.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anu365-my.sharepoint.com/personal/u6420297_anu_edu_au/Documents/ANU/PhD/Glass Fibre testing/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawm\VSCode Projects\GlassMechAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC10489CE99C46DE5BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A17A298-EE05-4A40-95DF-32E336C9FB6D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29A6A36D-EE09-484D-8FFB-22FEC975B7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
   <si>
     <t>test_num</t>
   </si>
@@ -376,6 +376,15 @@
   </si>
   <si>
     <t>A 6</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>favimat</t>
+  </si>
+  <si>
+    <t>instron</t>
   </si>
 </sst>
 </file>
@@ -712,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+      <selection activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,10 +733,10 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="9" width="15.77734375" customWidth="1"/>
+    <col min="6" max="10" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,13 +762,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -784,11 +796,14 @@
       <c r="H2">
         <v>21.594158152105603</v>
       </c>
-      <c r="J2">
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -813,11 +828,14 @@
       <c r="H3">
         <v>26.066110693145063</v>
       </c>
-      <c r="J3">
+      <c r="I3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -842,11 +860,14 @@
       <c r="H4">
         <v>24.94492104370029</v>
       </c>
-      <c r="J4">
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -871,11 +892,14 @@
       <c r="H5">
         <v>41.311729947835417</v>
       </c>
-      <c r="J5">
+      <c r="I5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -901,13 +925,16 @@
         <v>65.394998895016101</v>
       </c>
       <c r="I6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -932,11 +959,14 @@
       <c r="H7">
         <v>25.082338613260362</v>
       </c>
-      <c r="J7">
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -961,11 +991,14 @@
       <c r="H8">
         <v>25.707579985348239</v>
       </c>
-      <c r="J8">
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -990,11 +1023,14 @@
       <c r="H9">
         <v>21.08434245619274</v>
       </c>
-      <c r="J9">
+      <c r="I9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1020,13 +1056,16 @@
         <v>22.862520565210851</v>
       </c>
       <c r="I10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" t="s">
         <v>19</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1051,11 +1090,14 @@
       <c r="H11">
         <v>22.88066438059986</v>
       </c>
-      <c r="J11">
+      <c r="I11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1081,13 +1123,16 @@
         <v>29.270179379141904</v>
       </c>
       <c r="I12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" t="s">
         <v>19</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>14</v>
       </c>
@@ -1112,11 +1157,14 @@
       <c r="H13">
         <v>26.905943325371005</v>
       </c>
-      <c r="J13">
+      <c r="I13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>15</v>
       </c>
@@ -1142,13 +1190,16 @@
         <v>70.075043264159291</v>
       </c>
       <c r="I14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" t="s">
         <v>14</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>17</v>
       </c>
@@ -1173,11 +1224,14 @@
       <c r="H15">
         <v>24.758985355391612</v>
       </c>
-      <c r="J15">
+      <c r="I15" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>18</v>
       </c>
@@ -1202,11 +1256,14 @@
       <c r="H16">
         <v>25.714706523989104</v>
       </c>
-      <c r="J16">
+      <c r="I16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>19</v>
       </c>
@@ -1231,11 +1288,14 @@
       <c r="H17">
         <v>29.12360457413147</v>
       </c>
-      <c r="J17">
+      <c r="I17" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20</v>
       </c>
@@ -1260,11 +1320,14 @@
       <c r="H18">
         <v>26.250619559679848</v>
       </c>
-      <c r="J18">
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+      <c r="K18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1289,11 +1352,14 @@
       <c r="H19">
         <v>27.104134927958121</v>
       </c>
-      <c r="J19">
+      <c r="I19" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -1319,13 +1385,16 @@
         <v>27.993875423027184</v>
       </c>
       <c r="I20" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" t="s">
         <v>19</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15</v>
       </c>
@@ -1350,11 +1419,14 @@
       <c r="H21">
         <v>31.5644754538984</v>
       </c>
-      <c r="J21">
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+      <c r="K21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
@@ -1379,12 +1451,15 @@
       <c r="H22">
         <v>23.5457785309762</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22">
+      <c r="I22" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>17</v>
       </c>
@@ -1409,12 +1484,15 @@
       <c r="H23">
         <v>28.069649315094384</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23">
+      <c r="I23" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
@@ -1439,11 +1517,14 @@
       <c r="H24">
         <v>29.090362762393777</v>
       </c>
-      <c r="J24">
+      <c r="I24" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1468,11 +1549,14 @@
       <c r="H25">
         <v>29.758806538197135</v>
       </c>
-      <c r="J25">
+      <c r="I25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1497,11 +1581,14 @@
       <c r="H26">
         <v>27.607217016561663</v>
       </c>
-      <c r="J26">
+      <c r="I26" t="s">
+        <v>114</v>
+      </c>
+      <c r="K26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1526,11 +1613,14 @@
       <c r="H27">
         <v>25.454124184719092</v>
       </c>
-      <c r="J27">
+      <c r="I27" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1555,11 +1645,14 @@
       <c r="H28">
         <v>24.469824116475465</v>
       </c>
-      <c r="J28">
+      <c r="I28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1584,11 +1677,14 @@
       <c r="H29">
         <v>14.06223218890819</v>
       </c>
-      <c r="J29">
+      <c r="I29" t="s">
+        <v>114</v>
+      </c>
+      <c r="K29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1613,11 +1709,14 @@
       <c r="H30">
         <v>22.698020546351628</v>
       </c>
-      <c r="J30">
+      <c r="I30" t="s">
+        <v>114</v>
+      </c>
+      <c r="K30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1642,11 +1741,14 @@
       <c r="H31">
         <v>35.954754188306111</v>
       </c>
-      <c r="J31">
+      <c r="I31" t="s">
+        <v>114</v>
+      </c>
+      <c r="K31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1671,11 +1773,14 @@
       <c r="H32">
         <v>25.841981625179663</v>
       </c>
-      <c r="J32">
+      <c r="I32" t="s">
+        <v>114</v>
+      </c>
+      <c r="K32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -1700,11 +1805,14 @@
       <c r="H33">
         <v>27.323267542671847</v>
       </c>
-      <c r="J33">
+      <c r="I33" t="s">
+        <v>114</v>
+      </c>
+      <c r="K33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>19</v>
       </c>
@@ -1729,11 +1837,14 @@
       <c r="H34">
         <v>24.435472130301214</v>
       </c>
-      <c r="J34">
+      <c r="I34" t="s">
+        <v>114</v>
+      </c>
+      <c r="K34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1759,8 +1870,11 @@
       <c r="H35" s="6">
         <v>32.252038189113591</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1786,8 +1900,11 @@
       <c r="H36" s="6">
         <v>26.963167015998369</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I36" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>7</v>
       </c>
@@ -1813,8 +1930,11 @@
       <c r="H37" s="6">
         <v>25.246929866657489</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -1840,8 +1960,11 @@
       <c r="H38" s="6">
         <v>28.584503410928303</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I38" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>9</v>
       </c>
@@ -1867,8 +1990,11 @@
       <c r="H39" s="6">
         <v>26.152900044242092</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I39" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10</v>
       </c>
@@ -1894,8 +2020,11 @@
       <c r="H40" s="6">
         <v>29.924169062852872</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I40" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>11</v>
       </c>
@@ -1921,8 +2050,11 @@
       <c r="H41" s="6">
         <v>27.544668393322667</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I41" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>12</v>
       </c>
@@ -1948,8 +2080,11 @@
       <c r="H42" s="6">
         <v>33.701030538416305</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I42" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>14</v>
       </c>
@@ -1975,8 +2110,11 @@
       <c r="H43" s="6">
         <v>28.469024237080394</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I43" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
@@ -2002,8 +2140,11 @@
       <c r="H44" s="6">
         <v>26.820030596378835</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I44" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>17</v>
       </c>
@@ -2029,8 +2170,11 @@
       <c r="H45" s="6">
         <v>29.693921116269149</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I45" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>21</v>
       </c>
@@ -2056,8 +2200,11 @@
       <c r="H46" s="6">
         <v>28.432601363934481</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I46" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>23</v>
       </c>
@@ -2083,8 +2230,11 @@
       <c r="H47" s="6">
         <v>31.684490179081724</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I47" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>25</v>
       </c>
@@ -2110,8 +2260,11 @@
       <c r="H48" s="6">
         <v>33.500656963366666</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>29</v>
       </c>
@@ -2137,8 +2290,11 @@
       <c r="H49" s="6">
         <v>26.210357822661191</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>31</v>
       </c>
@@ -2164,8 +2320,11 @@
       <c r="H50" s="6">
         <v>25.537505618334997</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>34</v>
       </c>
@@ -2191,8 +2350,11 @@
       <c r="H51" s="6">
         <v>31.221896966321825</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>38</v>
       </c>
@@ -2218,8 +2380,11 @@
       <c r="H52" s="6">
         <v>31.797657777950075</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>46</v>
       </c>
@@ -2245,8 +2410,11 @@
       <c r="H53" s="6">
         <v>31.070829899463174</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2272,8 +2440,11 @@
       <c r="H54" s="6">
         <v>20.494718060550284</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>41</v>
       </c>
@@ -2299,8 +2470,11 @@
       <c r="H55" s="6">
         <v>20.881142527977424</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
@@ -2326,8 +2500,11 @@
       <c r="H56" s="6">
         <v>17.659460456064075</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5</v>
       </c>
@@ -2353,8 +2530,11 @@
       <c r="H57" s="6">
         <v>17.126798471190362</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6</v>
       </c>
@@ -2380,8 +2560,11 @@
       <c r="H58" s="6">
         <v>20.132157638933169</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>13</v>
       </c>
@@ -2407,8 +2590,11 @@
       <c r="H59" s="6">
         <v>13.76403983</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>19</v>
       </c>
@@ -2434,8 +2620,11 @@
       <c r="H60" s="6">
         <v>15.554052872301762</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>20</v>
       </c>
@@ -2461,8 +2650,11 @@
       <c r="H61" s="6">
         <v>20.333076705810427</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>22</v>
       </c>
@@ -2488,8 +2680,11 @@
       <c r="H62" s="6">
         <v>19.3058217626035</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>24</v>
       </c>
@@ -2515,8 +2710,11 @@
       <c r="H63" s="6">
         <v>19.713424079999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>26</v>
       </c>
@@ -2542,8 +2740,11 @@
       <c r="H64" s="6">
         <v>18.269771120969601</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>27</v>
       </c>
@@ -2569,8 +2770,11 @@
       <c r="H65" s="6">
         <v>16.691279120000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>30</v>
       </c>
@@ -2596,8 +2800,11 @@
       <c r="H66" s="6">
         <v>15.92657653730703</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>32</v>
       </c>
@@ -2623,8 +2830,11 @@
       <c r="H67" s="6">
         <v>16.424021348958828</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>33</v>
       </c>
@@ -2650,8 +2860,11 @@
       <c r="H68" s="6">
         <v>16.647920838877177</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I68" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>35</v>
       </c>
@@ -2677,8 +2890,11 @@
       <c r="H69" s="6">
         <v>19.223406479568439</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>36</v>
       </c>
@@ -2704,8 +2920,11 @@
       <c r="H70" s="6">
         <v>18.792476109232506</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I70" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>37</v>
       </c>
@@ -2731,8 +2950,11 @@
       <c r="H71" s="6">
         <v>15.209573968864451</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>42</v>
       </c>
@@ -2758,8 +2980,11 @@
       <c r="H72" s="6">
         <v>18.995662746255732</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>83</v>
       </c>
@@ -2778,8 +3003,11 @@
       <c r="H73" s="6">
         <v>22.176682848007978</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>84</v>
       </c>
@@ -2798,8 +3026,11 @@
       <c r="H74" s="6">
         <v>21.068753910865912</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>85</v>
       </c>
@@ -2818,8 +3049,11 @@
       <c r="H75" s="6">
         <v>20.413788597658286</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>86</v>
       </c>
@@ -2838,8 +3072,11 @@
       <c r="H76" s="6">
         <v>17.14447943614557</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>87</v>
       </c>
@@ -2858,8 +3095,11 @@
       <c r="H77" s="6">
         <v>20.748205473341834</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>88</v>
       </c>
@@ -2878,8 +3118,11 @@
       <c r="H78" s="6">
         <v>20.644062741044163</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>89</v>
       </c>
@@ -2898,8 +3141,11 @@
       <c r="H79" s="6">
         <v>18.487127468855263</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>90</v>
       </c>
@@ -2918,8 +3164,11 @@
       <c r="H80" s="6">
         <v>16.834797305496142</v>
       </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>91</v>
       </c>
@@ -2938,8 +3187,11 @@
       <c r="H81" s="6">
         <v>17.433486174601189</v>
       </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>92</v>
       </c>
@@ -2958,8 +3210,11 @@
       <c r="H82" s="6">
         <v>17.733756347407969</v>
       </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>93</v>
       </c>
@@ -2978,8 +3233,11 @@
       <c r="H83" s="6">
         <v>25.784364040262606</v>
       </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I83" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>94</v>
       </c>
@@ -2998,8 +3256,11 @@
       <c r="H84" s="6">
         <v>24.193507973413883</v>
       </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>95</v>
       </c>
@@ -3018,8 +3279,11 @@
       <c r="H85" s="6">
         <v>24.960974073635771</v>
       </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>96</v>
       </c>
@@ -3039,8 +3303,11 @@
       <c r="H86" s="6">
         <v>24.226382895819203</v>
       </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I86" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>97</v>
       </c>
@@ -3060,8 +3327,11 @@
       <c r="H87" s="6">
         <v>29.767682131711567</v>
       </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I87" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>98</v>
       </c>
@@ -3081,8 +3351,11 @@
       <c r="H88" s="6">
         <v>28.764518502713592</v>
       </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I88" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>99</v>
       </c>
@@ -3102,8 +3375,11 @@
       <c r="H89" s="6">
         <v>32.31573290692598</v>
       </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I89" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>100</v>
       </c>
@@ -3123,8 +3399,11 @@
       <c r="H90" s="6">
         <v>25.231275508386602</v>
       </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I90" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>101</v>
       </c>
@@ -3144,8 +3423,11 @@
       <c r="H91" s="6">
         <v>22.161352981139068</v>
       </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I91" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>97</v>
       </c>
@@ -3165,8 +3447,11 @@
       <c r="H92" s="6">
         <v>25.810365121258489</v>
       </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I92" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>102</v>
       </c>
@@ -3186,8 +3471,11 @@
       <c r="H93" s="6">
         <v>29.300197116378072</v>
       </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I93" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>103</v>
       </c>
@@ -3207,8 +3495,11 @@
       <c r="H94" s="6">
         <v>28.238980685964901</v>
       </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I94" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>98</v>
       </c>
@@ -3228,8 +3519,11 @@
       <c r="H95" s="6">
         <v>25.35499046132497</v>
       </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I95" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>104</v>
       </c>
@@ -3249,8 +3543,11 @@
       <c r="H96" s="6">
         <v>22.962666191832824</v>
       </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I96" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>105</v>
       </c>
@@ -3270,8 +3567,11 @@
       <c r="H97" s="6">
         <v>24.460075709265517</v>
       </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I97" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>106</v>
       </c>
@@ -3291,8 +3591,11 @@
       <c r="H98" s="6">
         <v>22.791580620688187</v>
       </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I98" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>107</v>
       </c>
@@ -3312,8 +3615,11 @@
       <c r="H99" s="6">
         <v>6.9046815176846152</v>
       </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I99" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>108</v>
       </c>
@@ -3333,8 +3639,11 @@
       <c r="H100" s="6">
         <v>4.7766448072144421</v>
       </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I100" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>109</v>
       </c>
@@ -3354,8 +3663,11 @@
       <c r="H101" s="6">
         <v>3.1235457135457123</v>
       </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I101" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>110</v>
       </c>
@@ -3375,8 +3687,11 @@
       <c r="H102" s="6">
         <v>3.4223828197945836</v>
       </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I102" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>111</v>
       </c>
@@ -3396,8 +3711,11 @@
       <c r="H103" s="6">
         <v>3.2482967032967052</v>
       </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I103" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>111</v>
       </c>
@@ -3417,8 +3735,11 @@
       <c r="H104" s="6">
         <v>3.771833763506387</v>
       </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I104" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>112</v>
       </c>
@@ -3437,6 +3758,9 @@
       </c>
       <c r="H105" s="6">
         <v>4.1912240725918188</v>
+      </c>
+      <c r="I105" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>